<commit_message>
Tạo Folder Activty, Update UseCase Format Tìm kiếm
</commit_message>
<xml_diff>
--- a/Phân tích/UseCases/5. Tìm kiếm.xlsx
+++ b/Phân tích/UseCases/5. Tìm kiếm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025AAC89-FB90-4BBE-9230-7F0C03E29538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087EDAEA-F0B6-42E9-BCB7-20FCA598CB1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04392538-DB61-43EC-AFA3-E88B6D995574}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>5. Actor nhập từ khóa vào thanh tìm kiếm</t>
   </si>
   <si>
-    <t>6. Hệ thống truy suất CSDL và hiện kết quả ra màn hình</t>
-  </si>
-  <si>
     <t>Tìm kiếm</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>3. Actor chọn chức năng cần sử dụng (quản lí nhân viên, đơn đặt hàng, khách hàng, kho, hóa đơn)</t>
+  </si>
+  <si>
+    <t>6. Hệ thống truy xuất CSDL và hiện kết quả ra màn hình</t>
   </si>
 </sst>
 </file>
@@ -205,21 +205,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -236,6 +236,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>499532</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>50990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E287A23D-CAB1-4D59-9BDF-5B603FA7F53A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6502400"/>
+          <a:ext cx="2836332" cy="6942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E5EAC9-BCA6-4B31-A937-E7944D29B1E5}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,49 +601,49 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="3"/>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3"/>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="3"/>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -605,145 +654,145 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="3"/>
+      <c r="B21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="3"/>
+      <c r="B24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="6"/>
       <c r="E25" t="s">
         <v>24</v>
       </c>
@@ -752,19 +801,19 @@
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="3"/>
+      <c r="B26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="7">
         <v>44159</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -788,5 +837,6 @@
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Quản lí hệ thống
</commit_message>
<xml_diff>
--- a/Phân tích/UseCases/5. Tìm kiếm.xlsx
+++ b/Phân tích/UseCases/5. Tìm kiếm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4096A12D-74DE-4C29-838F-829EF2BABF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2590B4CD-542F-4A3C-B55A-5A54367AFEE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04392538-DB61-43EC-AFA3-E88B6D995574}"/>
   </bookViews>
@@ -170,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,11 +193,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -220,6 +255,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -244,13 +288,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2142067</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>60490</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -628,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E5EAC9-BCA6-4B31-A937-E7944D29B1E5}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,133 +796,117 @@
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C22" s="6"/>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B24" s="7">
         <v>44159</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C24" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
+  <mergeCells count="17">
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>